<commit_message>
Added more code and updates
</commit_message>
<xml_diff>
--- a/Data/clean/Scorecards Clean - Faye's Version.xlsx
+++ b/Data/clean/Scorecards Clean - Faye's Version.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cefayefang/Library/CloudStorage/Box-Box/Legislative Scorecards/Data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96964652-59E1-7E4D-AEC1-35B7E58D0EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD03332F-A339-784C-86F3-9CD666E652C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6600" yWindow="760" windowWidth="23640" windowHeight="18880" activeTab="1" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="315">
   <si>
     <t>Year</t>
   </si>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78E89D-5764-1045-B6D6-35D1F0809A40}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="137" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1724,6 +1724,9 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
+      <c r="F13" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2016,6 +2019,9 @@
       </c>
       <c r="E29" t="s">
         <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding Emily's arizona code and further example code.
</commit_message>
<xml_diff>
--- a/Data/clean/Scorecards Clean - Faye's Version.xlsx
+++ b/Data/clean/Scorecards Clean - Faye's Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cefayefang/Library/CloudStorage/Box-Box/Legislative Scorecards/Data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD03332F-A339-784C-86F3-9CD666E652C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353E9C85-572A-DC4C-B966-8944BCA00E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6600" yWindow="760" windowWidth="23640" windowHeight="18880" activeTab="1" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="316">
   <si>
     <t>Year</t>
   </si>
@@ -983,6 +983,9 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>Water Score</t>
   </si>
 </sst>
 </file>
@@ -1467,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78E89D-5764-1045-B6D6-35D1F0809A40}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="137" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2431,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0734319C-46E1-6B43-95CA-FBADA7542208}">
-  <dimension ref="A1:N182"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2452,7 +2455,7 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2495,8 +2498,11 @@
       <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -2587,7 +2593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>38</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2717,7 +2723,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
finish wyoming and add all codes/fix some potential error in score calculation code
</commit_message>
<xml_diff>
--- a/Data/clean/Scorecards Clean - Faye's Version.xlsx
+++ b/Data/clean/Scorecards Clean - Faye's Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cefayefang/Library/CloudStorage/Box-Box/Legislative Scorecards/Data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353E9C85-572A-DC4C-B966-8944BCA00E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A5FA8-D57F-4441-A772-A1558CE289F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="760" windowWidth="23640" windowHeight="18880" activeTab="1" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
+    <workbookView xWindow="2960" yWindow="760" windowWidth="23640" windowHeight="18880" activeTab="1" xr2:uid="{EFE6F266-E20E-3A47-983A-491ECE3CE1FF}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="315">
   <si>
     <t>Year</t>
   </si>
@@ -914,9 +914,6 @@
   </si>
   <si>
     <t>Ray</t>
-  </si>
-  <si>
-    <t>HB 24—Subsidies for Local Predator Contro</t>
   </si>
   <si>
     <t>HB 32—Game and Fish Electronic Licensing</t>
@@ -1470,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C78E89D-5764-1045-B6D6-35D1F0809A40}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2024,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2126,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -2146,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2163,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -2183,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -2203,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
@@ -2220,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -2240,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2260,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2277,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E44" t="s">
         <v>11</v>
@@ -2297,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E45" t="s">
         <v>11</v>
@@ -2317,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E46" t="s">
         <v>11</v>
@@ -2337,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -2357,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
@@ -2374,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -2397,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
@@ -2406,7 +2403,7 @@
         <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2420,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -2499,7 +2496,7 @@
         <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -3964,7 +3961,7 @@
         <v>115</v>
       </c>
       <c r="E57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F57" t="s">
         <v>150</v>
@@ -3990,7 +3987,7 @@
         <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F58" t="s">
         <v>150</v>
@@ -4016,7 +4013,7 @@
         <v>117</v>
       </c>
       <c r="E59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F59" t="s">
         <v>150</v>
@@ -4088,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
+        <v>307</v>
+      </c>
+      <c r="E62" t="s">
         <v>308</v>
-      </c>
-      <c r="E62" t="s">
-        <v>309</v>
       </c>
       <c r="F62" t="s">
         <v>150</v>
@@ -4310,7 +4307,7 @@
         <v>128</v>
       </c>
       <c r="E71" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F71" t="s">
         <v>153</v>
@@ -4590,7 +4587,7 @@
         <v>138</v>
       </c>
       <c r="E82" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F82" t="s">
         <v>150</v>
@@ -4639,7 +4636,7 @@
         <v>140</v>
       </c>
       <c r="E84" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F84" t="s">
         <v>150</v>
@@ -5470,7 +5467,7 @@
         <v>115</v>
       </c>
       <c r="E118" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F118" t="s">
         <v>150</v>
@@ -5496,7 +5493,7 @@
         <v>116</v>
       </c>
       <c r="E119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F119" t="s">
         <v>150</v>
@@ -5522,7 +5519,7 @@
         <v>117</v>
       </c>
       <c r="E120" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F120" t="s">
         <v>150</v>
@@ -5594,10 +5591,10 @@
         <v>0</v>
       </c>
       <c r="D123" t="s">
+        <v>307</v>
+      </c>
+      <c r="E123" t="s">
         <v>308</v>
-      </c>
-      <c r="E123" t="s">
-        <v>309</v>
       </c>
       <c r="F123" t="s">
         <v>150</v>
@@ -5813,7 +5810,7 @@
         <v>128</v>
       </c>
       <c r="E132" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F132" t="s">
         <v>153</v>
@@ -6093,7 +6090,7 @@
         <v>138</v>
       </c>
       <c r="E143" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F143" t="s">
         <v>150</v>

</xml_diff>